<commit_message>
esquema de BBDD terminado
</commit_message>
<xml_diff>
--- a/BaseDeDatos-OpenSport.xlsx
+++ b/BaseDeDatos-OpenSport.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleay\Google Drive\Programación\Proyecto Integrador\proyectointegrador\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BA18E49-1571-4F63-A1C7-5FCB8EE65041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E02F5A2-6BAE-4F01-878B-366B3A7D9CA8}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20640" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>ALE</t>
   </si>
@@ -163,9 +157,6 @@
   </si>
   <si>
     <t>KEYWORD_PRODUCTO</t>
-  </si>
-  <si>
-    <t>KEYWORD_KEYWORD</t>
   </si>
   <si>
     <t>FAVORITO_PRODUCTO</t>
@@ -189,7 +180,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -945,33 +936,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5636327-9E85-4BB5-8F23-7F03D3AAF58D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1018,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>12</v>
       </c>
@@ -1063,7 +1054,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>14</v>
       </c>
@@ -1099,7 +1090,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>20</v>
       </c>
@@ -1121,7 +1112,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>23</v>
       </c>
@@ -1143,7 +1134,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>26</v>
       </c>
@@ -1165,7 +1156,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>29</v>
       </c>
@@ -1187,7 +1178,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>32</v>
       </c>
@@ -1205,7 +1196,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>33</v>
       </c>
@@ -1223,7 +1214,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
         <v>34</v>
       </c>
@@ -1241,7 +1232,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>35</v>
       </c>
@@ -1259,7 +1250,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>36</v>
       </c>
@@ -1277,7 +1268,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>37</v>
       </c>
@@ -1295,7 +1286,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>38</v>
       </c>
@@ -1313,7 +1304,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1329,7 +1320,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -1347,7 +1338,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
         <v>40</v>
       </c>
@@ -1360,22 +1351,19 @@
       <c r="D18" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
         <v>12</v>
       </c>
@@ -1391,79 +1379,70 @@
       <c r="E19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="32"/>
       <c r="C22" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="5"/>
@@ -1477,7 +1456,7 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="6"/>
       <c r="C23" s="15" t="s">
@@ -1495,7 +1474,7 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="5"/>
@@ -1511,7 +1490,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>

</xml_diff>

<commit_message>
incorporacion de fetch y correciones de validacion
</commit_message>
<xml_diff>
--- a/BaseDeDatos-OpenSport.xlsx
+++ b/BaseDeDatos-OpenSport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleay\Google Drive\Programación\Proyecto Integrador\proyectointegrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BA18E49-1571-4F63-A1C7-5FCB8EE65041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47383D5C-C0CD-46A8-9E81-0142819BBC25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E02F5A2-6BAE-4F01-878B-366B3A7D9CA8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>ALE</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>SILVI</t>
-  </si>
-  <si>
-    <t>MARCA_PRODUCTO</t>
   </si>
   <si>
     <t>CATEGORIA_PRODUCTO</t>
@@ -190,7 +187,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +208,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -538,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -561,12 +565,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -627,17 +625,50 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -955,9 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5636327-9E85-4BB5-8F23-7F03D3AAF58D}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -992,35 +1021,35 @@
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="16" t="s">
         <v>11</v>
       </c>
       <c r="L2" s="2"/>
@@ -1028,35 +1057,35 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="23" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="20" t="s">
         <v>12</v>
       </c>
       <c r="L3" s="2"/>
@@ -1064,35 +1093,35 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="13" t="s">
         <v>19</v>
       </c>
       <c r="L4" s="2"/>
@@ -1100,98 +1129,98 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="24" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
       <c r="L5" s="2"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="24" t="s">
+      <c r="F6" s="19"/>
+      <c r="G6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
       <c r="L6" s="2"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="24" t="s">
+      <c r="F7" s="19"/>
+      <c r="G7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
       <c r="L7" s="2"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="25" t="s">
+      <c r="F8" s="19"/>
+      <c r="G8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
       <c r="L8" s="2"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1206,7 +1235,7 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="2"/>
@@ -1224,7 +1253,7 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="25" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="2"/>
@@ -1242,7 +1271,7 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="2"/>
@@ -1260,7 +1289,7 @@
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="2"/>
@@ -1278,7 +1307,7 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="2"/>
@@ -1296,7 +1325,7 @@
       <c r="N14" s="1"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="2"/>
@@ -1347,24 +1376,21 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="30" t="s">
+    <row r="18" spans="1:14" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="29" t="s">
         <v>43</v>
       </c>
       <c r="E18" s="30" t="s">
         <v>44</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>45</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="1"/>
@@ -1376,22 +1402,19 @@
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="13" t="s">
+      <c r="E19" s="32" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="2"/>
@@ -1404,23 +1427,20 @@
       <c r="N19" s="1"/>
     </row>
     <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="9" t="s">
+      <c r="A20" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="34" t="s">
         <v>47</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>48</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="1"/>
@@ -1432,23 +1452,20 @@
       <c r="N20" s="1"/>
     </row>
     <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>49</v>
+      <c r="A21" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>48</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="1"/>
@@ -1460,14 +1477,13 @@
       <c r="N21" s="1"/>
     </row>
     <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="38"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1478,14 +1494,13 @@
       <c r="N22" s="1"/>
     </row>
     <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="15" t="s">
+      <c r="A23" s="40"/>
+      <c r="B23" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>

</xml_diff>

<commit_message>
base de datos completa
</commit_message>
<xml_diff>
--- a/BaseDeDatos-OpenSport.xlsx
+++ b/BaseDeDatos-OpenSport.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleay\Google Drive\Programación\Proyecto Integrador\proyectointegrador\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47383D5C-C0CD-46A8-9E81-0142819BBC25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E02F5A2-6BAE-4F01-878B-366B3A7D9CA8}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20640" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>ALE</t>
   </si>
@@ -160,9 +154,6 @@
   </si>
   <si>
     <t>KEYWORD_PRODUCTO</t>
-  </si>
-  <si>
-    <t>KEYWORD_KEYWORD</t>
   </si>
   <si>
     <t>FAVORITO_PRODUCTO</t>
@@ -186,7 +177,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -976,31 +967,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5636327-9E85-4BB5-8F23-7F03D3AAF58D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1049,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
@@ -1092,7 +1085,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>14</v>
       </c>
@@ -1128,7 +1121,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>20</v>
       </c>
@@ -1150,7 +1143,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>23</v>
       </c>
@@ -1172,7 +1165,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>26</v>
       </c>
@@ -1194,7 +1187,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>29</v>
       </c>
@@ -1216,7 +1209,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>32</v>
       </c>
@@ -1234,7 +1227,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>33</v>
       </c>
@@ -1252,7 +1245,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>34</v>
       </c>
@@ -1270,7 +1263,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>35</v>
       </c>
@@ -1288,7 +1281,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>36</v>
       </c>
@@ -1306,7 +1299,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>37</v>
       </c>
@@ -1324,7 +1317,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>38</v>
       </c>
@@ -1342,7 +1335,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1358,7 +1351,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -1376,7 +1369,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
         <v>40</v>
       </c>
@@ -1386,22 +1379,19 @@
       <c r="C18" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
         <v>12</v>
       </c>
@@ -1414,72 +1404,63 @@
       <c r="D19" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="34" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37"/>
       <c r="B22" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="38"/>
       <c r="D22" s="39"/>
@@ -1493,7 +1474,7 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="40"/>
       <c r="B23" s="36" t="s">
         <v>27</v>
@@ -1510,7 +1491,7 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="5"/>
@@ -1526,7 +1507,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>

</xml_diff>